<commit_message>
dashboard meal show by user
</commit_message>
<xml_diff>
--- a/Sample Data.xlsx
+++ b/Sample Data.xlsx
@@ -990,19 +990,19 @@
   <sheetPr/>
   <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="W20" sqref="W20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="16.3" customWidth="1"/>
-    <col min="2" max="2" width="4" customWidth="1"/>
-    <col min="3" max="3" width="2.4" customWidth="1"/>
-    <col min="4" max="4" width="2.9" customWidth="1"/>
+    <col min="2" max="2" width="4.5" customWidth="1"/>
+    <col min="3" max="3" width="3.1" customWidth="1"/>
+    <col min="4" max="4" width="3.5" customWidth="1"/>
     <col min="5" max="5" width="3.9" customWidth="1"/>
-    <col min="6" max="6" width="2.2" customWidth="1"/>
-    <col min="7" max="7" width="2.9" customWidth="1"/>
+    <col min="6" max="6" width="2.7" customWidth="1"/>
+    <col min="7" max="7" width="3.9" customWidth="1"/>
     <col min="8" max="8" width="2.6" customWidth="1"/>
     <col min="9" max="9" width="2.5" customWidth="1"/>
     <col min="10" max="10" width="2.9" customWidth="1"/>
@@ -1011,7 +1011,7 @@
     <col min="13" max="13" width="2.8" customWidth="1"/>
     <col min="14" max="14" width="2.1" customWidth="1"/>
     <col min="15" max="15" width="2.5" customWidth="1"/>
-    <col min="16" max="16" width="3" customWidth="1"/>
+    <col min="16" max="16" width="3.8" customWidth="1"/>
     <col min="21" max="21" width="13.9" customWidth="1"/>
     <col min="22" max="22" width="9.3"/>
   </cols>

</xml_diff>

<commit_message>
reckoning total meals, bazaar, extra cost user wise show and total meals, bazaar, extra cost, meal rate, extra cost per member calculation shows
</commit_message>
<xml_diff>
--- a/Sample Data.xlsx
+++ b/Sample Data.xlsx
@@ -51,9 +51,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
@@ -65,9 +65,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -81,6 +88,43 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -98,6 +142,38 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -105,31 +181,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -142,60 +194,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -218,187 +218,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -409,6 +409,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -423,50 +447,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -486,17 +466,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -509,162 +494,180 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="distributed" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -991,7 +994,7 @@
   <dimension ref="A1:Y17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75"/>
@@ -1022,71 +1025,71 @@
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="2">
+      <c r="E1" s="3">
         <v>2</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2">
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3">
         <v>3</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2">
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3">
         <v>4</v>
       </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2">
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3">
         <v>5</v>
       </c>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
     </row>
     <row r="2" spans="2:16">
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="H2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K2" t="s">
-        <v>0</v>
-      </c>
-      <c r="L2" t="s">
-        <v>1</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="K2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="N2" t="s">
-        <v>0</v>
-      </c>
-      <c r="O2" t="s">
-        <v>1</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="N2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1094,49 +1097,49 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
         <v>0.5</v>
       </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1</v>
+      </c>
+      <c r="H3" s="2">
         <v>0.5</v>
       </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3">
+      <c r="I3" s="2">
+        <v>1</v>
+      </c>
+      <c r="J3" s="2">
+        <v>1</v>
+      </c>
+      <c r="K3" s="2">
         <v>0.5</v>
       </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
+      <c r="L3" s="2">
+        <v>0</v>
+      </c>
+      <c r="M3" s="2">
+        <v>0</v>
+      </c>
+      <c r="N3" s="2">
         <v>0.5</v>
       </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3">
+      <c r="O3" s="2">
+        <v>0</v>
+      </c>
+      <c r="P3" s="2">
         <v>0</v>
       </c>
       <c r="Q3">
@@ -1148,49 +1151,49 @@
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>0.5</v>
       </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2">
         <v>0.5</v>
       </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
+      <c r="I4" s="2">
+        <v>1</v>
+      </c>
+      <c r="J4" s="2">
+        <v>1</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0</v>
+      </c>
+      <c r="L4" s="2">
+        <v>1</v>
+      </c>
+      <c r="M4" s="2">
+        <v>0</v>
+      </c>
+      <c r="N4" s="2">
         <v>0.5</v>
       </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4">
+      <c r="O4" s="2">
+        <v>0</v>
+      </c>
+      <c r="P4" s="2">
         <v>0</v>
       </c>
       <c r="Q4">
@@ -1203,16 +1206,16 @@
         <f>SUM(Q3:Q4)</f>
         <v>15.5</v>
       </c>
-      <c r="S5" s="2" t="s">
+      <c r="S5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="T5" s="2"/>
-      <c r="U5" s="2"/>
-      <c r="W5" s="2" t="s">
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="W5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="X5" s="2"/>
-      <c r="Y5" s="2"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
     </row>
     <row r="6" spans="19:25">
       <c r="S6" t="s">

</xml_diff>